<commit_message>
1. Added new citations and parties spreadsheets.  2. Updated spreadsheets based upon latest.  3. Reset cim/json outputs.
</commit_message>
<xml_diff>
--- a/cmip6/models/ipsl-cm6a-atm-hr/cmip6_ipsl_ipsl-cm6a-atm-hr_land.xlsx
+++ b/cmip6/models/ipsl-cm6a-atm-hr/cmip6_ipsl_ipsl-cm6a-atm-hr_land.xlsx
@@ -123,7 +123,7 @@
     <t>STRING</t>
   </si>
   <si>
-    <t>Mnemonic references to responsible parties</t>
+    <t>Responsible party identifiers</t>
   </si>
   <si>
     <t>NOTE: Multiple entries are allowed, please insert a new row per entry.</t>
@@ -135,7 +135,7 @@
     <t>Citations</t>
   </si>
   <si>
-    <t>Mnemonic references to citations</t>
+    <t>Citation identifiers</t>
   </si>
   <si>
     <t>2.1</t>

</xml_diff>